<commit_message>
Updates Write data into excel
</commit_message>
<xml_diff>
--- a/SeleniumWebDriver/testdata/TestDataWrite.xlsx
+++ b/SeleniumWebDriver/testdata/TestDataWrite.xlsx
@@ -6,21 +6,57 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" r:id="rId3" sheetId="1"/>
+    <sheet name="Sheet1" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
-    <t>Welcome</t>
+    <t>BookName</t>
   </si>
   <si>
-    <t>TO</t>
+    <t>PurchesedDate</t>
   </si>
   <si>
-    <t>Java</t>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>selenium</t>
+  </si>
+  <si>
+    <t>29-Jul-2024</t>
+  </si>
+  <si>
+    <t>350.0</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>java</t>
+  </si>
+  <si>
+    <t>200.0</t>
+  </si>
+  <si>
+    <t>python</t>
+  </si>
+  <si>
+    <t>250.0</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>150.0</t>
   </si>
 </sst>
 </file>
@@ -65,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -81,6 +117,65 @@
       <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
+      <c r="D1" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>